<commit_message>
Heuristicas top 12 banco e  projetos em Java
</commit_message>
<xml_diff>
--- a/resources/annotated.xlsx
+++ b/resources/annotated.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leomurta/workspace/db-mining/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilapaiva/Documents/GitHub/db-mining/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F6F013-6321-A946-947D-C5F8D7AE65F4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7380" yWindow="2140" windowWidth="28800" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="2019-08-23" sheetId="1" r:id="rId1"/>
@@ -19,11 +18,17 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2019-08-23'!$A$1:$W$1110</definedName>
     <definedName name="Z_5C673459_04D6_4823_9839_02892B7E791C_.wvu.FilterData" localSheetId="0" hidden="1">'2019-08-23'!$U$1:$U$1112</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <customWorkbookViews>
     <customWorkbookView name="Filter 1" guid="{5C673459-04D6-4823-9839-02892B7E791C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -3157,7 +3162,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
@@ -3549,12 +3554,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD1112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="S2" sqref="S2:S390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3717,7 +3722,7 @@
         <v>21</v>
       </c>
       <c r="S2" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A2),"/"),B2)</f>
+        <f>CONCATENATE(CONCATENATE(CONCATENATE("http://www.github.com/",A2),"/"),B2)</f>
         <v>http://www.github.com/activeadmin/activeadmin</v>
       </c>
       <c r="T2" s="6" t="s">
@@ -3794,7 +3799,7 @@
         <v>23</v>
       </c>
       <c r="S3" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A3),"/"),B3)</f>
+        <f t="shared" ref="S3:S66" si="0">CONCATENATE(CONCATENATE(CONCATENATE("http://www.github.com/",A3),"/"),B3)</f>
         <v>http://www.github.com/Activiti/Activiti</v>
       </c>
       <c r="T3" s="6" t="s">
@@ -3871,7 +3876,7 @@
         <v>0</v>
       </c>
       <c r="S4" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A4),"/"),B4)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/adambard/learnxinyminutes-docs</v>
       </c>
       <c r="T4" s="6" t="s">
@@ -3948,7 +3953,7 @@
         <v>67</v>
       </c>
       <c r="S5" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A5),"/"),B5)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/adobe/brackets</v>
       </c>
       <c r="T5" s="6" t="s">
@@ -4025,7 +4030,7 @@
         <v>17</v>
       </c>
       <c r="S6" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A6),"/"),B6)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/aframevr/aframe</v>
       </c>
       <c r="T6" s="6" t="s">
@@ -4102,7 +4107,7 @@
         <v>159</v>
       </c>
       <c r="S7" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A7),"/"),B7)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/ag-grid/ag-grid</v>
       </c>
       <c r="T7" s="6" t="s">
@@ -4179,7 +4184,7 @@
         <v>113</v>
       </c>
       <c r="S8" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A8),"/"),B8)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/aio-libs/aiohttp</v>
       </c>
       <c r="T8" s="6" t="s">
@@ -4256,7 +4261,7 @@
         <v>0</v>
       </c>
       <c r="S9" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A9),"/"),B9)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/ajaxorg/ace</v>
       </c>
       <c r="T9" s="6" t="s">
@@ -4333,7 +4338,7 @@
         <v>31</v>
       </c>
       <c r="S10" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A10),"/"),B10)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/alibaba/druid</v>
       </c>
       <c r="T10" s="8" t="s">
@@ -4410,7 +4415,7 @@
         <v>488</v>
       </c>
       <c r="S11" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A11),"/"),B11)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/ampproject/amphtml</v>
       </c>
       <c r="T11" s="6" t="s">
@@ -4487,7 +4492,7 @@
         <v>0</v>
       </c>
       <c r="S12" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A12),"/"),B12)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/angular/angular</v>
       </c>
       <c r="T12" s="6" t="s">
@@ -4564,7 +4569,7 @@
         <v>0</v>
       </c>
       <c r="S13" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A13),"/"),B13)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/angular/angular.js</v>
       </c>
       <c r="T13" s="6" t="s">
@@ -4641,7 +4646,7 @@
         <v>106</v>
       </c>
       <c r="S14" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A14),"/"),B14)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/angular/components</v>
       </c>
       <c r="T14" s="6" t="s">
@@ -4718,7 +4723,7 @@
         <v>3</v>
       </c>
       <c r="S15" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A15),"/"),B15)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/ansible/ansible</v>
       </c>
       <c r="T15" s="6" t="s">
@@ -4795,7 +4800,7 @@
         <v>0</v>
       </c>
       <c r="S16" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A16),"/"),B16)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/ansible/awx</v>
       </c>
       <c r="T16" s="6" t="s">
@@ -4872,7 +4877,7 @@
         <v>268</v>
       </c>
       <c r="S17" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A17),"/"),B17)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/ant-design/ant-design</v>
       </c>
       <c r="T17" s="6" t="s">
@@ -4949,7 +4954,7 @@
         <v>0</v>
       </c>
       <c r="S18" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A18),"/"),B18)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/antirez/redis</v>
       </c>
       <c r="T18" s="6" t="s">
@@ -5026,7 +5031,7 @@
         <v>18</v>
       </c>
       <c r="S19" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A19),"/"),B19)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/antlr/antlr4</v>
       </c>
       <c r="T19" s="6" t="s">
@@ -5103,7 +5108,7 @@
         <v>10</v>
       </c>
       <c r="S20" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A20),"/"),B20)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/apache/airflow</v>
       </c>
       <c r="T20" s="6" t="s">
@@ -5180,7 +5185,7 @@
         <v>0</v>
       </c>
       <c r="S21" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A21),"/"),B21)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/apache/cassandra</v>
       </c>
       <c r="T21" s="6" t="s">
@@ -5257,7 +5262,7 @@
         <v>0</v>
       </c>
       <c r="S22" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A22),"/"),B22)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/apache/flink</v>
       </c>
       <c r="T22" s="6" t="s">
@@ -5334,7 +5339,7 @@
         <v>0</v>
       </c>
       <c r="S23" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A23),"/"),B23)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/apache/hadoop</v>
       </c>
       <c r="T23" s="6" t="s">
@@ -5411,7 +5416,7 @@
         <v>34</v>
       </c>
       <c r="S24" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A24),"/"),B24)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/apache/incubator-druid</v>
       </c>
       <c r="T24" s="6" t="s">
@@ -5488,7 +5493,7 @@
         <v>57</v>
       </c>
       <c r="S25" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A25),"/"),B25)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/apache/incubator-echarts</v>
       </c>
       <c r="T25" s="6" t="s">
@@ -5565,7 +5570,7 @@
         <v>18</v>
       </c>
       <c r="S26" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A26),"/"),B26)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/apache/incubator-mxnet</v>
       </c>
       <c r="T26" s="6" t="s">
@@ -5642,7 +5647,7 @@
         <v>35</v>
       </c>
       <c r="S27" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A27),"/"),B27)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/apache/incubator-shardingsphere</v>
       </c>
       <c r="T27" s="6" t="s">
@@ -5719,7 +5724,7 @@
         <v>4</v>
       </c>
       <c r="S28" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A28),"/"),B28)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/apache/incubator-weex</v>
       </c>
       <c r="T28" s="6" t="s">
@@ -5796,7 +5801,7 @@
         <v>0</v>
       </c>
       <c r="S29" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A29),"/"),B29)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/apache/kafka</v>
       </c>
       <c r="T29" s="8" t="s">
@@ -5873,7 +5878,7 @@
         <v>33</v>
       </c>
       <c r="S30" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A30),"/"),B30)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/apache/skywalking</v>
       </c>
       <c r="T30" s="6" t="s">
@@ -5950,7 +5955,7 @@
         <v>0</v>
       </c>
       <c r="S31" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A31),"/"),B31)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/apache/storm</v>
       </c>
       <c r="T31" s="6" t="s">
@@ -6027,7 +6032,7 @@
         <v>2</v>
       </c>
       <c r="S32" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A32),"/"),B32)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/apache/thrift</v>
       </c>
       <c r="T32" s="6" t="s">
@@ -6104,7 +6109,7 @@
         <v>134</v>
       </c>
       <c r="S33" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A33),"/"),B33)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/apereo/cas</v>
       </c>
       <c r="T33" s="6" t="s">
@@ -6181,7 +6186,7 @@
         <v>7</v>
       </c>
       <c r="S34" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A34),"/"),B34)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/ApolloAuto/apollo</v>
       </c>
       <c r="T34" s="6" t="s">
@@ -6258,7 +6263,7 @@
         <v>0</v>
       </c>
       <c r="S35" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A35),"/"),B35)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/apollographql/apollo-client</v>
       </c>
       <c r="T35" s="6" t="s">
@@ -6335,7 +6340,7 @@
         <v>96</v>
       </c>
       <c r="S36" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A36),"/"),B36)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/appium/appium</v>
       </c>
       <c r="T36" s="6" t="s">
@@ -6412,7 +6417,7 @@
         <v>60</v>
       </c>
       <c r="S37" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A37),"/"),B37)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/apple/foundationdb</v>
       </c>
       <c r="T37" s="6" t="s">
@@ -6489,7 +6494,7 @@
         <v>16</v>
       </c>
       <c r="S38" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A38),"/"),B38)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/apple/swift</v>
       </c>
       <c r="T38" s="6" t="s">
@@ -6566,7 +6571,7 @@
         <v>0</v>
       </c>
       <c r="S39" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A39),"/"),B39)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/arangodb/arangodb</v>
       </c>
       <c r="T39" s="6" t="s">
@@ -6643,7 +6648,7 @@
         <v>27</v>
       </c>
       <c r="S40" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A40),"/"),B40)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/arduino/Arduino</v>
       </c>
       <c r="T40" s="8" t="s">
@@ -6720,7 +6725,7 @@
         <v>21</v>
       </c>
       <c r="S41" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A41),"/"),B41)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/aria2/aria2</v>
       </c>
       <c r="T41" s="6" t="s">
@@ -6797,7 +6802,7 @@
         <v>46</v>
       </c>
       <c r="S42" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A42),"/"),B42)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/aseprite/aseprite</v>
       </c>
       <c r="T42" s="6" t="s">
@@ -6874,7 +6879,7 @@
         <v>58</v>
       </c>
       <c r="S43" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A43),"/"),B43)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/aspnet/AspNetCore</v>
       </c>
       <c r="T43" s="6" t="s">
@@ -6951,7 +6956,7 @@
         <v>8</v>
       </c>
       <c r="S44" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A44),"/"),B44)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/aspnet/AspNetCore.Docs</v>
       </c>
       <c r="T44" s="6" t="s">
@@ -7028,7 +7033,7 @@
         <v>52</v>
       </c>
       <c r="S45" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A45),"/"),B45)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/aspnet/EntityFrameworkCore</v>
       </c>
       <c r="T45" s="6" t="s">
@@ -7105,7 +7110,7 @@
         <v>185</v>
       </c>
       <c r="S46" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A46),"/"),B46)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/aspnetboilerplate/aspnetboilerplate</v>
       </c>
       <c r="T46" s="6" t="s">
@@ -7182,7 +7187,7 @@
         <v>0</v>
       </c>
       <c r="S47" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A47),"/"),B47)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/astaxie/build-web-application-with-golang</v>
       </c>
       <c r="T47" s="6" t="s">
@@ -7259,7 +7264,7 @@
         <v>498</v>
       </c>
       <c r="S48" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A48),"/"),B48)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/atom/atom</v>
       </c>
       <c r="T48" s="6" t="s">
@@ -7336,7 +7341,7 @@
         <v>57</v>
       </c>
       <c r="S49" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A49),"/"),B49)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/AudioKit/AudioKit</v>
       </c>
       <c r="T49" s="6" t="s">
@@ -7413,7 +7418,7 @@
         <v>5</v>
       </c>
       <c r="S50" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A50),"/"),B50)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/Automattic/mongoose</v>
       </c>
       <c r="T50" s="6" t="s">
@@ -7490,7 +7495,7 @@
         <v>10</v>
       </c>
       <c r="S51" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A51),"/"),B51)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/Automattic/wp-calypso</v>
       </c>
       <c r="T51" s="6" t="s">
@@ -7567,7 +7572,7 @@
         <v>7</v>
       </c>
       <c r="S52" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A52),"/"),B52)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/AvaloniaUI/Avalonia</v>
       </c>
       <c r="T52" s="6" t="s">
@@ -7644,7 +7649,7 @@
         <v>0</v>
       </c>
       <c r="S53" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A53),"/"),B53)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/avwo/whistle</v>
       </c>
       <c r="T53" s="6" t="s">
@@ -7721,7 +7726,7 @@
         <v>1</v>
       </c>
       <c r="S54" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A54),"/"),B54)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/aws/aws-cli</v>
       </c>
       <c r="T54" s="6" t="s">
@@ -7798,7 +7803,7 @@
         <v>33</v>
       </c>
       <c r="S55" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A55),"/"),B55)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/b3log/symphony</v>
       </c>
       <c r="T55" s="6" t="s">
@@ -7875,7 +7880,7 @@
         <v>175</v>
       </c>
       <c r="S56" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A56),"/"),B56)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/babel/babel</v>
       </c>
       <c r="T56" s="6" t="s">
@@ -7952,7 +7957,7 @@
         <v>47</v>
       </c>
       <c r="S57" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A57),"/"),B57)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/BabylonJS/Babylon.js</v>
       </c>
       <c r="T57" s="8" t="s">
@@ -8029,7 +8034,7 @@
         <v>35</v>
       </c>
       <c r="S58" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A58),"/"),B58)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/balderdashy/sails</v>
       </c>
       <c r="T58" s="6" t="s">
@@ -8106,7 +8111,7 @@
         <v>71</v>
       </c>
       <c r="S59" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A59),"/"),B59)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/bazelbuild/bazel</v>
       </c>
       <c r="T59" s="6" t="s">
@@ -8183,7 +8188,7 @@
         <v>0</v>
       </c>
       <c r="S60" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A60),"/"),B60)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/bcit-ci/CodeIgniter</v>
       </c>
       <c r="T60" s="6" t="s">
@@ -8260,7 +8265,7 @@
         <v>31</v>
       </c>
       <c r="S61" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A61),"/"),B61)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/beetbox/beets</v>
       </c>
       <c r="T61" s="6" t="s">
@@ -8337,7 +8342,7 @@
         <v>29</v>
       </c>
       <c r="S62" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A62),"/"),B62)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/bitcoin/bitcoin</v>
       </c>
       <c r="T62" s="6" t="s">
@@ -8414,7 +8419,7 @@
         <v>0</v>
       </c>
       <c r="S63" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A63),"/"),B63)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/bkaradzic/bgfx</v>
       </c>
       <c r="T63" s="6" t="s">
@@ -8491,7 +8496,7 @@
         <v>0</v>
       </c>
       <c r="S64" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A64),"/"),B64)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/bokeh/bokeh</v>
       </c>
       <c r="T64" s="6" t="s">
@@ -8568,7 +8573,7 @@
         <v>58</v>
       </c>
       <c r="S65" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A65),"/"),B65)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/borgbackup/borg</v>
       </c>
       <c r="T65" s="6" t="s">
@@ -8645,7 +8650,7 @@
         <v>0</v>
       </c>
       <c r="S66" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A66),"/"),B66)</f>
+        <f t="shared" si="0"/>
         <v>http://www.github.com/boto/boto</v>
       </c>
       <c r="T66" s="6" t="s">
@@ -8722,7 +8727,7 @@
         <v>19</v>
       </c>
       <c r="S67" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A67),"/"),B67)</f>
+        <f t="shared" ref="S67:S130" si="1">CONCATENATE(CONCATENATE(CONCATENATE("http://www.github.com/",A67),"/"),B67)</f>
         <v>http://www.github.com/botpress/botpress</v>
       </c>
       <c r="T67" s="6" t="s">
@@ -8799,7 +8804,7 @@
         <v>5</v>
       </c>
       <c r="S68" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A68),"/"),B68)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/bulletphysics/bullet3</v>
       </c>
       <c r="T68" s="6" t="s">
@@ -8876,7 +8881,7 @@
         <v>54</v>
       </c>
       <c r="S69" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A69),"/"),B69)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/CachetHQ/Cachet</v>
       </c>
       <c r="T69" s="6" t="s">
@@ -8953,7 +8958,7 @@
         <v>281</v>
       </c>
       <c r="S70" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A70),"/"),B70)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/cakephp/cakephp</v>
       </c>
       <c r="T70" s="6" t="s">
@@ -9030,7 +9035,7 @@
         <v>0</v>
       </c>
       <c r="S71" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A71),"/"),B71)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/ccxt/ccxt</v>
       </c>
       <c r="T71" s="6" t="s">
@@ -9107,7 +9112,7 @@
         <v>74</v>
       </c>
       <c r="S72" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A72),"/"),B72)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/cefsharp/CefSharp</v>
       </c>
       <c r="T72" s="6" t="s">
@@ -9184,7 +9189,7 @@
         <v>1</v>
       </c>
       <c r="S73" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A73),"/"),B73)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/celery/celery</v>
       </c>
       <c r="T73" s="6" t="s">
@@ -9261,7 +9266,7 @@
         <v>0</v>
       </c>
       <c r="S74" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A74),"/"),B74)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/ceph/ceph</v>
       </c>
       <c r="T74" s="6" t="s">
@@ -9338,7 +9343,7 @@
         <v>0</v>
       </c>
       <c r="S75" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A75),"/"),B75)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/certbot/certbot</v>
       </c>
       <c r="T75" s="6" t="s">
@@ -9415,7 +9420,7 @@
         <v>18</v>
       </c>
       <c r="S76" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A76),"/"),B76)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/Chatie/wechaty</v>
       </c>
       <c r="T76" s="6" t="s">
@@ -9492,7 +9497,7 @@
         <v>3</v>
       </c>
       <c r="S77" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A77),"/"),B77)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/chef/chef</v>
       </c>
       <c r="T77" s="6" t="s">
@@ -9569,7 +9574,7 @@
         <v>0</v>
       </c>
       <c r="S78" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A78),"/"),B78)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/citra-emu/citra</v>
       </c>
       <c r="T78" s="6" t="s">
@@ -9646,7 +9651,7 @@
         <v>17</v>
       </c>
       <c r="S79" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A79),"/"),B79)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/cockroachdb/cockroach</v>
       </c>
       <c r="T79" s="6" t="s">
@@ -9723,7 +9728,7 @@
         <v>153</v>
       </c>
       <c r="S80" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A80),"/"),B80)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/CocoaPods/CocoaPods</v>
       </c>
       <c r="T80" s="6" t="s">
@@ -9800,7 +9805,7 @@
         <v>0</v>
       </c>
       <c r="S81" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A81),"/"),B81)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/cocos2d/cocos2d-x</v>
       </c>
       <c r="T81" s="6" t="s">
@@ -9877,7 +9882,7 @@
         <v>121</v>
       </c>
       <c r="S82" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A82),"/"),B82)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/codemirror/CodeMirror</v>
       </c>
       <c r="T82" s="6" t="s">
@@ -9954,7 +9959,7 @@
         <v>64</v>
       </c>
       <c r="S83" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A83),"/"),B83)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/composer/composer</v>
       </c>
       <c r="T83" s="6" t="s">
@@ -10031,7 +10036,7 @@
         <v>28</v>
       </c>
       <c r="S84" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A84),"/"),B84)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/CRYTEK/CRYENGINE</v>
       </c>
       <c r="T84" s="6" t="s">
@@ -10108,7 +10113,7 @@
         <v>0</v>
       </c>
       <c r="S85" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A85),"/"),B85)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/cucumber/cucumber-ruby</v>
       </c>
       <c r="T85" s="6" t="s">
@@ -10185,7 +10190,7 @@
         <v>38</v>
       </c>
       <c r="S86" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A86),"/"),B86)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/curl/curl</v>
       </c>
       <c r="T86" s="6" t="s">
@@ -10262,7 +10267,7 @@
         <v>0</v>
       </c>
       <c r="S87" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A87),"/"),B87)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/dask/dask</v>
       </c>
       <c r="T87" s="6" t="s">
@@ -10339,7 +10344,7 @@
         <v>18</v>
       </c>
       <c r="S88" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A88),"/"),B88)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/davisking/dlib</v>
       </c>
       <c r="T88" s="6" t="s">
@@ -10416,7 +10421,7 @@
         <v>86</v>
       </c>
       <c r="S89" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A89),"/"),B89)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/dbeaver/dbeaver</v>
       </c>
       <c r="T89" s="6" t="s">
@@ -10493,7 +10498,7 @@
         <v>0</v>
       </c>
       <c r="S90" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A90),"/"),B90)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/DefinitelyTyped/DefinitelyTyped</v>
       </c>
       <c r="T90" s="6" t="s">
@@ -10570,7 +10575,7 @@
         <v>0</v>
       </c>
       <c r="S91" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A91),"/"),B91)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/desktop/desktop</v>
       </c>
       <c r="T91" s="6" t="s">
@@ -10647,7 +10652,7 @@
         <v>0</v>
       </c>
       <c r="S92" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A92),"/"),B92)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/dianping/cat</v>
       </c>
       <c r="T92" s="6" t="s">
@@ -10724,7 +10729,7 @@
         <v>82</v>
       </c>
       <c r="S93" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A93),"/"),B93)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/diaspora/diaspora</v>
       </c>
       <c r="T93" s="6" t="s">
@@ -10801,7 +10806,7 @@
         <v>0</v>
       </c>
       <c r="S94" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A94),"/"),B94)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/discourse/discourse</v>
       </c>
       <c r="T94" s="6" t="s">
@@ -10878,7 +10883,7 @@
         <v>33</v>
       </c>
       <c r="S95" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A95),"/"),B95)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/DivanteLtd/vue-storefront</v>
       </c>
       <c r="T95" s="6" t="s">
@@ -10955,7 +10960,7 @@
         <v>0</v>
       </c>
       <c r="S96" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A96),"/"),B96)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/divio/django-cms</v>
       </c>
       <c r="T96" s="6" t="s">
@@ -11032,7 +11037,7 @@
         <v>0</v>
       </c>
       <c r="S97" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A97),"/"),B97)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/django/django</v>
       </c>
       <c r="T97" s="6" t="s">
@@ -11109,7 +11114,7 @@
         <v>111</v>
       </c>
       <c r="S98" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A98),"/"),B98)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/docker/compose</v>
       </c>
       <c r="T98" s="6" t="s">
@@ -11186,7 +11191,7 @@
         <v>30</v>
       </c>
       <c r="S99" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A99),"/"),B99)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/doctrine/dbal</v>
       </c>
       <c r="T99" s="6" t="s">
@@ -11263,7 +11268,7 @@
         <v>30</v>
       </c>
       <c r="S100" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A100),"/"),B100)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/doctrine/orm</v>
       </c>
       <c r="T100" s="6" t="s">
@@ -11340,7 +11345,7 @@
         <v>0</v>
       </c>
       <c r="S101" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A101),"/"),B101)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/dolphin-emu/dolphin</v>
       </c>
       <c r="T101" s="6" t="s">
@@ -11417,7 +11422,7 @@
         <v>71</v>
       </c>
       <c r="S102" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A102),"/"),B102)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/dotnet/coreclr</v>
       </c>
       <c r="T102" s="6" t="s">
@@ -11494,7 +11499,7 @@
         <v>73</v>
       </c>
       <c r="S103" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A103),"/"),B103)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/dotnet/corefx</v>
       </c>
       <c r="T103" s="6" t="s">
@@ -11571,7 +11576,7 @@
         <v>38</v>
       </c>
       <c r="S104" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A104),"/"),B104)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/dotnet/roslyn</v>
       </c>
       <c r="T104" s="6" t="s">
@@ -11648,7 +11653,7 @@
         <v>66</v>
       </c>
       <c r="S105" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A105),"/"),B105)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/dropwizard/dropwizard</v>
       </c>
       <c r="T105" s="6" t="s">
@@ -11725,7 +11730,7 @@
         <v>12</v>
       </c>
       <c r="S106" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A106),"/"),B106)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/eclipse/che</v>
       </c>
       <c r="T106" s="6" t="s">
@@ -11802,7 +11807,7 @@
         <v>125</v>
       </c>
       <c r="S107" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A107),"/"),B107)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/elastic/beats</v>
       </c>
       <c r="T107" s="6" t="s">
@@ -11879,7 +11884,7 @@
         <v>6</v>
       </c>
       <c r="S108" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A108),"/"),B108)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/elastic/elasticsearch</v>
       </c>
       <c r="T108" s="6" t="s">
@@ -11956,7 +11961,7 @@
         <v>7</v>
       </c>
       <c r="S109" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A109),"/"),B109)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/elastic/kibana</v>
       </c>
       <c r="T109" s="6" t="s">
@@ -12033,7 +12038,7 @@
         <v>6</v>
       </c>
       <c r="S110" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A110),"/"),B110)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/elastic/logstash</v>
       </c>
       <c r="T110" s="6" t="s">
@@ -12110,7 +12115,7 @@
         <v>464</v>
       </c>
       <c r="S111" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A111),"/"),B111)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/electron/electron</v>
       </c>
       <c r="T111" s="6" t="s">
@@ -12187,7 +12192,7 @@
         <v>264</v>
       </c>
       <c r="S112" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A112),"/"),B112)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/emberjs/ember.js</v>
       </c>
       <c r="T112" s="6" t="s">
@@ -12264,7 +12269,7 @@
         <v>0</v>
       </c>
       <c r="S113" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A113),"/"),B113)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/emscripten-core/emscripten</v>
       </c>
       <c r="T113" s="6" t="s">
@@ -12341,7 +12346,7 @@
         <v>13</v>
       </c>
       <c r="S114" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A114),"/"),B114)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/encode/django-rest-framework</v>
       </c>
       <c r="T114" s="6" t="s">
@@ -12418,7 +12423,7 @@
         <v>76</v>
       </c>
       <c r="S115" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A115),"/"),B115)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/EOSIO/eos</v>
       </c>
       <c r="T115" s="6" t="s">
@@ -12495,7 +12500,7 @@
         <v>193</v>
       </c>
       <c r="S116" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A116),"/"),B116)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/eslint/eslint</v>
       </c>
       <c r="T116" s="6" t="s">
@@ -12572,7 +12577,7 @@
         <v>161</v>
       </c>
       <c r="S117" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A117),"/"),B117)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/etcd-io/etcd</v>
       </c>
       <c r="T117" s="6" t="s">
@@ -12649,7 +12654,7 @@
         <v>20</v>
       </c>
       <c r="S118" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A118),"/"),B118)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/ether/etherpad-lite</v>
       </c>
       <c r="T118" s="6" t="s">
@@ -12726,7 +12731,7 @@
         <v>115</v>
       </c>
       <c r="S119" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A119),"/"),B119)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/ethereum/go-ethereum</v>
       </c>
       <c r="T119" s="6" t="s">
@@ -12803,7 +12808,7 @@
         <v>55</v>
       </c>
       <c r="S120" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A120),"/"),B120)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/ethereum/solidity</v>
       </c>
       <c r="T120" s="6" t="s">
@@ -12880,7 +12885,7 @@
         <v>0</v>
       </c>
       <c r="S121" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A121),"/"),B121)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/eugenp/tutorials</v>
       </c>
       <c r="T121" s="6" t="s">
@@ -12957,7 +12962,7 @@
         <v>59</v>
       </c>
       <c r="S122" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A122),"/"),B122)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/explosion/spaCy</v>
       </c>
       <c r="T122" s="6" t="s">
@@ -13034,7 +13039,7 @@
         <v>140</v>
       </c>
       <c r="S123" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A123),"/"),B123)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/expressjs/express</v>
       </c>
       <c r="T123" s="6" t="s">
@@ -13111,7 +13116,7 @@
         <v>46</v>
       </c>
       <c r="S124" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A124),"/"),B124)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/facebook/buck</v>
       </c>
       <c r="T124" s="6" t="s">
@@ -13188,7 +13193,7 @@
         <v>0</v>
       </c>
       <c r="S125" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A125),"/"),B125)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/facebook/folly</v>
       </c>
       <c r="T125" s="6" t="s">
@@ -13265,7 +13270,7 @@
         <v>15</v>
       </c>
       <c r="S126" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A126),"/"),B126)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/facebook/hhvm</v>
       </c>
       <c r="T126" s="8" t="s">
@@ -13342,7 +13347,7 @@
         <v>36</v>
       </c>
       <c r="S127" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A127),"/"),B127)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/facebook/litho</v>
       </c>
       <c r="T127" s="6" t="s">
@@ -13419,7 +13424,7 @@
         <v>83</v>
       </c>
       <c r="S128" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A128),"/"),B128)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/facebook/react</v>
       </c>
       <c r="T128" s="6" t="s">
@@ -13496,7 +13501,7 @@
         <v>127</v>
       </c>
       <c r="S129" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A129),"/"),B129)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/facebook/react-native</v>
       </c>
       <c r="T129" s="6" t="s">
@@ -13573,7 +13578,7 @@
         <v>112</v>
       </c>
       <c r="S130" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A130),"/"),B130)</f>
+        <f t="shared" si="1"/>
         <v>http://www.github.com/facebook/rocksdb</v>
       </c>
       <c r="T130" s="6" t="s">
@@ -13650,7 +13655,7 @@
         <v>56</v>
       </c>
       <c r="S131" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A131),"/"),B131)</f>
+        <f t="shared" ref="S131:S194" si="2">CONCATENATE(CONCATENATE(CONCATENATE("http://www.github.com/",A131),"/"),B131)</f>
         <v>http://www.github.com/facebook/zstd</v>
       </c>
       <c r="T131" s="6" t="s">
@@ -13727,7 +13732,7 @@
         <v>408</v>
       </c>
       <c r="S132" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A132),"/"),B132)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/fastlane/fastlane</v>
       </c>
       <c r="T132" s="6" t="s">
@@ -13804,7 +13809,7 @@
         <v>11</v>
       </c>
       <c r="S133" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A133),"/"),B133)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/FFmpeg/FFmpeg</v>
       </c>
       <c r="T133" s="6" t="s">
@@ -13881,7 +13886,7 @@
         <v>0</v>
       </c>
       <c r="S134" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A134),"/"),B134)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/flynn/flynn</v>
       </c>
       <c r="T134" s="6" t="s">
@@ -13958,7 +13963,7 @@
         <v>29</v>
       </c>
       <c r="S135" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A135),"/"),B135)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/FormidableLabs/victory</v>
       </c>
       <c r="T135" s="6" t="s">
@@ -14035,7 +14040,7 @@
         <v>35</v>
       </c>
       <c r="S136" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A136),"/"),B136)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/Foundry376/Mailspring</v>
       </c>
       <c r="T136" s="6" t="s">
@@ -14112,7 +14117,7 @@
         <v>807</v>
       </c>
       <c r="S137" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A137),"/"),B137)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/frappe/erpnext</v>
       </c>
       <c r="T137" s="6" t="s">
@@ -14189,7 +14194,7 @@
         <v>0</v>
       </c>
       <c r="S138" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A138),"/"),B138)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/freeCodeCamp/freeCodeCamp</v>
       </c>
       <c r="T138" s="6" t="s">
@@ -14266,7 +14271,7 @@
         <v>114</v>
       </c>
       <c r="S139" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A139),"/"),B139)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/FriendsOfPHP/PHP-CS-Fixer</v>
       </c>
       <c r="T139" s="6" t="s">
@@ -14343,7 +14348,7 @@
         <v>74</v>
       </c>
       <c r="S140" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A140),"/"),B140)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/gatsbyjs/gatsby</v>
       </c>
       <c r="T140" s="6" t="s">
@@ -14420,7 +14425,7 @@
         <v>178</v>
       </c>
       <c r="S141" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A141),"/"),B141)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/getgrav/grav</v>
       </c>
       <c r="T141" s="6" t="s">
@@ -14497,7 +14502,7 @@
         <v>84</v>
       </c>
       <c r="S142" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A142),"/"),B142)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/getlantern/lantern</v>
       </c>
       <c r="T142" s="6" t="s">
@@ -14574,7 +14579,7 @@
         <v>92</v>
       </c>
       <c r="S143" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A143),"/"),B143)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/getredash/redash</v>
       </c>
       <c r="T143" s="6" t="s">
@@ -14651,7 +14656,7 @@
         <v>52</v>
       </c>
       <c r="S144" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A144),"/"),B144)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/getsentry/sentry</v>
       </c>
       <c r="T144" s="6" t="s">
@@ -14728,7 +14733,7 @@
         <v>0</v>
       </c>
       <c r="S145" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A145),"/"),B145)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/giampaolo/psutil</v>
       </c>
       <c r="T145" s="6" t="s">
@@ -14805,7 +14810,7 @@
         <v>0</v>
       </c>
       <c r="S146" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A146),"/"),B146)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/git/git</v>
       </c>
       <c r="T146" s="6" t="s">
@@ -14882,7 +14887,7 @@
         <v>71</v>
       </c>
       <c r="S147" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A147),"/"),B147)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/git-lfs/git-lfs</v>
       </c>
       <c r="T147" s="6" t="s">
@@ -14959,7 +14964,7 @@
         <v>95</v>
       </c>
       <c r="S148" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A148),"/"),B148)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/github/linguist</v>
       </c>
       <c r="T148" s="6" t="s">
@@ -15036,7 +15041,7 @@
         <v>0</v>
       </c>
       <c r="S149" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A149),"/"),B149)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/gitlabhq/gitlabhq</v>
       </c>
       <c r="T149" s="6" t="s">
@@ -15113,7 +15118,7 @@
         <v>66</v>
       </c>
       <c r="S150" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A150),"/"),B150)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/go-gitea/gitea</v>
       </c>
       <c r="T150" s="6" t="s">
@@ -15190,7 +15195,7 @@
         <v>51</v>
       </c>
       <c r="S151" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A151),"/"),B151)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/gocd/gocd</v>
       </c>
       <c r="T151" s="6" t="s">
@@ -15267,7 +15272,7 @@
         <v>23</v>
       </c>
       <c r="S152" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A152),"/"),B152)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/godotengine/godot</v>
       </c>
       <c r="T152" s="6" t="s">
@@ -15344,7 +15349,7 @@
         <v>56</v>
       </c>
       <c r="S153" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A153),"/"),B153)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/gogs/gogs</v>
       </c>
       <c r="T153" s="6" t="s">
@@ -15421,7 +15426,7 @@
         <v>68</v>
       </c>
       <c r="S154" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A154),"/"),B154)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/goharbor/harbor</v>
       </c>
       <c r="T154" s="6" t="s">
@@ -15498,7 +15503,7 @@
         <v>94</v>
       </c>
       <c r="S155" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A155),"/"),B155)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/gohugoio/hugo</v>
       </c>
       <c r="T155" s="6" t="s">
@@ -15575,7 +15580,7 @@
         <v>0</v>
       </c>
       <c r="S156" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A156),"/"),B156)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/golang/go</v>
       </c>
       <c r="T156" s="6" t="s">
@@ -15652,7 +15657,7 @@
         <v>1</v>
       </c>
       <c r="S157" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A157),"/"),B157)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/google/closure-compiler</v>
       </c>
       <c r="T157" s="6" t="s">
@@ -15729,7 +15734,7 @@
         <v>0</v>
       </c>
       <c r="S158" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A158),"/"),B158)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/google/ExoPlayer</v>
       </c>
       <c r="T158" s="6" t="s">
@@ -15806,7 +15811,7 @@
         <v>26</v>
       </c>
       <c r="S159" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A159),"/"),B159)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/google/guava</v>
       </c>
       <c r="T159" s="6" t="s">
@@ -15883,7 +15888,7 @@
         <v>158</v>
       </c>
       <c r="S160" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A160),"/"),B160)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/gorhill/uBlock</v>
       </c>
       <c r="T160" s="6" t="s">
@@ -15960,7 +15965,7 @@
         <v>141</v>
       </c>
       <c r="S161" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A161),"/"),B161)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/grafana/grafana</v>
       </c>
       <c r="T161" s="6" t="s">
@@ -16037,7 +16042,7 @@
         <v>119</v>
       </c>
       <c r="S162" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A162),"/"),B162)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/grpc/grpc</v>
       </c>
       <c r="T162" s="6" t="s">
@@ -16114,7 +16119,7 @@
         <v>70</v>
       </c>
       <c r="S163" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A163),"/"),B163)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/h2o/h2o</v>
       </c>
       <c r="T163" s="6" t="s">
@@ -16191,7 +16196,7 @@
         <v>543</v>
       </c>
       <c r="S164" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A164),"/"),B164)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/HabitRPG/habitica</v>
       </c>
       <c r="T164" s="6" t="s">
@@ -16268,7 +16273,7 @@
         <v>166</v>
       </c>
       <c r="S165" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A165),"/"),B165)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/handsontable/handsontable</v>
       </c>
       <c r="T165" s="6" t="s">
@@ -16345,7 +16350,7 @@
         <v>1</v>
       </c>
       <c r="S166" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A166),"/"),B166)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/hapijs/hapi</v>
       </c>
       <c r="T166" s="6" t="s">
@@ -16422,7 +16427,7 @@
         <v>14</v>
       </c>
       <c r="S167" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A167),"/"),B167)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/hashcat/hashcat</v>
       </c>
       <c r="T167" s="6" t="s">
@@ -16499,7 +16504,7 @@
         <v>0</v>
       </c>
       <c r="S168" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A168),"/"),B168)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/hashicorp/consul</v>
       </c>
       <c r="T168" s="8" t="s">
@@ -16576,7 +16581,7 @@
         <v>2</v>
       </c>
       <c r="S169" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A169),"/"),B169)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/hashicorp/nomad</v>
       </c>
       <c r="T169" s="6" t="s">
@@ -16653,7 +16658,7 @@
         <v>2</v>
       </c>
       <c r="S170" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A170),"/"),B170)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/hashicorp/packer</v>
       </c>
       <c r="T170" s="6" t="s">
@@ -16730,7 +16735,7 @@
         <v>98</v>
       </c>
       <c r="S171" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A171),"/"),B171)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/hashicorp/terraform</v>
       </c>
       <c r="T171" s="8" t="s">
@@ -16807,7 +16812,7 @@
         <v>0</v>
       </c>
       <c r="S172" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A172),"/"),B172)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/hashicorp/vagrant</v>
       </c>
       <c r="T172" s="6" t="s">
@@ -16884,7 +16889,7 @@
         <v>0</v>
       </c>
       <c r="S173" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A173),"/"),B173)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/hashicorp/vault</v>
       </c>
       <c r="T173" s="6" t="s">
@@ -16961,7 +16966,7 @@
         <v>0</v>
       </c>
       <c r="S174" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A174),"/"),B174)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/highcharts/highcharts</v>
       </c>
       <c r="T174" s="6" t="s">
@@ -17038,7 +17043,7 @@
         <v>0</v>
       </c>
       <c r="S175" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A175),"/"),B175)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/highlightjs/highlight.js</v>
       </c>
       <c r="T175" s="6" t="s">
@@ -17115,7 +17120,7 @@
         <v>442</v>
       </c>
       <c r="S176" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A176),"/"),B176)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/home-assistant/home-assistant</v>
       </c>
       <c r="T176" s="6" t="s">
@@ -17192,7 +17197,7 @@
         <v>115</v>
       </c>
       <c r="S177" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A177),"/"),B177)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/Homebrew/brew</v>
       </c>
       <c r="T177" s="6" t="s">
@@ -17269,7 +17274,7 @@
         <v>81</v>
       </c>
       <c r="S178" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A178),"/"),B178)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/Homebrew/homebrew-cask</v>
       </c>
       <c r="T178" s="6" t="s">
@@ -17346,7 +17351,7 @@
         <v>0</v>
       </c>
       <c r="S179" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A179),"/"),B179)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/Homebrew/homebrew-core</v>
       </c>
       <c r="T179" s="6" t="s">
@@ -17423,7 +17428,7 @@
         <v>0</v>
       </c>
       <c r="S180" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A180),"/"),B180)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/hyperledger/fabric</v>
       </c>
       <c r="T180" s="6" t="s">
@@ -17500,7 +17505,7 @@
         <v>32</v>
       </c>
       <c r="S181" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A181),"/"),B181)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/icsharpcode/ILSpy</v>
       </c>
       <c r="T181" s="6" t="s">
@@ -17577,7 +17582,7 @@
         <v>153</v>
       </c>
       <c r="S182" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A182),"/"),B182)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/infernojs/inferno</v>
       </c>
       <c r="T182" s="6" t="s">
@@ -17654,7 +17659,7 @@
         <v>20</v>
       </c>
       <c r="S183" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A183),"/"),B183)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/influxdata/influxdb</v>
       </c>
       <c r="T183" s="6" t="s">
@@ -17731,7 +17736,7 @@
         <v>161</v>
       </c>
       <c r="S184" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A184),"/"),B184)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/ionic-team/ionic</v>
       </c>
       <c r="T184" s="6" t="s">
@@ -17808,7 +17813,7 @@
         <v>7</v>
       </c>
       <c r="S185" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A185),"/"),B185)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/ipfs/go-ipfs</v>
       </c>
       <c r="T185" s="6" t="s">
@@ -17885,7 +17890,7 @@
         <v>26</v>
       </c>
       <c r="S186" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A186),"/"),B186)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/ipython/ipython</v>
       </c>
       <c r="T186" s="6" t="s">
@@ -17962,7 +17967,7 @@
         <v>74</v>
       </c>
       <c r="S187" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A187),"/"),B187)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/istio/istio</v>
       </c>
       <c r="T187" s="6" t="s">
@@ -18039,7 +18044,7 @@
         <v>41</v>
       </c>
       <c r="S188" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A188),"/"),B188)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/JeffreySu/WeiXinMPSDK</v>
       </c>
       <c r="T188" s="6" t="s">
@@ -18116,7 +18121,7 @@
         <v>93</v>
       </c>
       <c r="S189" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A189),"/"),B189)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/jekyll/jekyll</v>
       </c>
       <c r="T189" s="6" t="s">
@@ -18193,7 +18198,7 @@
         <v>2</v>
       </c>
       <c r="S190" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A190),"/"),B190)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/jenkinsci/jenkins</v>
       </c>
       <c r="T190" s="6" t="s">
@@ -18270,7 +18275,7 @@
         <v>0</v>
       </c>
       <c r="S191" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A191),"/"),B191)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/JetBrains/intellij-community</v>
       </c>
       <c r="T191" s="6" t="s">
@@ -18347,7 +18352,7 @@
         <v>0</v>
       </c>
       <c r="S192" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A192),"/"),B192)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/jhipster/generator-jhipster</v>
       </c>
       <c r="T192" s="6" t="s">
@@ -18424,7 +18429,7 @@
         <v>0</v>
       </c>
       <c r="S193" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A193),"/"),B193)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/jquery/jquery</v>
       </c>
       <c r="T193" s="6" t="s">
@@ -18501,7 +18506,7 @@
         <v>0</v>
       </c>
       <c r="S194" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A194),"/"),B194)</f>
+        <f t="shared" si="2"/>
         <v>http://www.github.com/jquery/jquery-mobile</v>
       </c>
       <c r="T194" s="6" t="s">
@@ -18578,7 +18583,7 @@
         <v>0</v>
       </c>
       <c r="S195" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A195),"/"),B195)</f>
+        <f t="shared" ref="S195:S258" si="3">CONCATENATE(CONCATENATE(CONCATENATE("http://www.github.com/",A195),"/"),B195)</f>
         <v>http://www.github.com/jquery/jquery-ui</v>
       </c>
       <c r="T195" s="6" t="s">
@@ -18655,7 +18660,7 @@
         <v>14</v>
       </c>
       <c r="S196" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A196),"/"),B196)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/jupyter/notebook</v>
       </c>
       <c r="T196" s="6" t="s">
@@ -18732,7 +18737,7 @@
         <v>18</v>
       </c>
       <c r="S197" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A197),"/"),B197)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/jupyterlab/jupyterlab</v>
       </c>
       <c r="T197" s="6" t="s">
@@ -18809,7 +18814,7 @@
         <v>20</v>
       </c>
       <c r="S198" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A198),"/"),B198)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/keras-team/keras</v>
       </c>
       <c r="T198" s="6" t="s">
@@ -18886,7 +18891,7 @@
         <v>65</v>
       </c>
       <c r="S199" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A199),"/"),B199)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/keybase/client</v>
       </c>
       <c r="T199" s="6" t="s">
@@ -18963,7 +18968,7 @@
         <v>16</v>
       </c>
       <c r="S200" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A200),"/"),B200)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/keystonejs/keystone</v>
       </c>
       <c r="T200" s="6" t="s">
@@ -19040,7 +19045,7 @@
         <v>6</v>
       </c>
       <c r="S201" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A201),"/"),B201)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/kivy/kivy</v>
       </c>
       <c r="T201" s="6" t="s">
@@ -19117,7 +19122,7 @@
         <v>157</v>
       </c>
       <c r="S202" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A202),"/"),B202)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/kovidgoyal/calibre</v>
       </c>
       <c r="T202" s="6" t="s">
@@ -19194,7 +19199,7 @@
         <v>58</v>
       </c>
       <c r="S203" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A203),"/"),B203)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/kubernetes/kops</v>
       </c>
       <c r="T203" s="8" t="s">
@@ -19271,7 +19276,7 @@
         <v>334</v>
       </c>
       <c r="S204" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A204),"/"),B204)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/kubernetes/kubernetes</v>
       </c>
       <c r="T204" s="6" t="s">
@@ -19348,7 +19353,7 @@
         <v>59</v>
       </c>
       <c r="S205" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A205),"/"),B205)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/kubernetes/minikube</v>
       </c>
       <c r="T205" s="6" t="s">
@@ -19425,7 +19430,7 @@
         <v>150</v>
       </c>
       <c r="S206" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A206),"/"),B206)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/laravel/framework</v>
       </c>
       <c r="T206" s="6" t="s">
@@ -19500,7 +19505,7 @@
         <v>21</v>
       </c>
       <c r="S207" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A207),"/"),B207)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/laravel/laravel</v>
       </c>
       <c r="T207" s="6" t="s">
@@ -19577,7 +19582,7 @@
         <v>20</v>
       </c>
       <c r="S208" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A208),"/"),B208)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/Leaflet/Leaflet</v>
       </c>
       <c r="T208" s="6" t="s">
@@ -19654,7 +19659,7 @@
         <v>3</v>
       </c>
       <c r="S209" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A209),"/"),B209)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/libgdx/libgdx</v>
       </c>
       <c r="T209" s="6" t="s">
@@ -19731,7 +19736,7 @@
         <v>63</v>
       </c>
       <c r="S210" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A210),"/"),B210)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/libgit2/libgit2</v>
       </c>
       <c r="T210" s="6" t="s">
@@ -19808,7 +19813,7 @@
         <v>6</v>
       </c>
       <c r="S211" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A211),"/"),B211)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/linuxkit/linuxkit</v>
       </c>
       <c r="T211" s="6" t="s">
@@ -19885,7 +19890,7 @@
         <v>2</v>
       </c>
       <c r="S212" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A212),"/"),B212)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/lodash/lodash</v>
       </c>
       <c r="T212" s="6" t="s">
@@ -19962,7 +19967,7 @@
         <v>94</v>
       </c>
       <c r="S213" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A213),"/"),B213)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/magento/magento2</v>
       </c>
       <c r="T213" s="6" t="s">
@@ -20039,7 +20044,7 @@
         <v>32</v>
       </c>
       <c r="S214" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A214),"/"),B214)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/MahApps/MahApps.Metro</v>
       </c>
       <c r="T214" s="6" t="s">
@@ -20116,7 +20121,7 @@
         <v>7</v>
       </c>
       <c r="S215" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A215),"/"),B215)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/mailpile/Mailpile</v>
       </c>
       <c r="T215" s="6" t="s">
@@ -20193,7 +20198,7 @@
         <v>22</v>
       </c>
       <c r="S216" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A216),"/"),B216)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/MarlinFirmware/Marlin</v>
       </c>
       <c r="T216" s="6" t="s">
@@ -20270,7 +20275,7 @@
         <v>96</v>
       </c>
       <c r="S217" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A217),"/"),B217)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/marmelab/react-admin</v>
       </c>
       <c r="T217" s="6" t="s">
@@ -20347,7 +20352,7 @@
         <v>1</v>
       </c>
       <c r="S218" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A218),"/"),B218)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/material-components/material-components-web</v>
       </c>
       <c r="T218" s="6" t="s">
@@ -20424,7 +20429,7 @@
         <v>425</v>
       </c>
       <c r="S219" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A219),"/"),B219)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/matomo-org/matomo</v>
       </c>
       <c r="T219" s="6" t="s">
@@ -20501,7 +20506,7 @@
         <v>37</v>
       </c>
       <c r="S220" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A220),"/"),B220)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/matplotlib/matplotlib</v>
       </c>
       <c r="T220" s="6" t="s">
@@ -20578,7 +20583,7 @@
         <v>154</v>
       </c>
       <c r="S221" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A221),"/"),B221)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/mattermost/mattermost-server</v>
       </c>
       <c r="T221" s="6" t="s">
@@ -20655,7 +20660,7 @@
         <v>231</v>
       </c>
       <c r="S222" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A222),"/"),B222)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/Maximus5/ConEmu</v>
       </c>
       <c r="T222" s="6" t="s">
@@ -20732,7 +20737,7 @@
         <v>0</v>
       </c>
       <c r="S223" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A223),"/"),B223)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/meteor/meteor</v>
       </c>
       <c r="T223" s="6" t="s">
@@ -20809,7 +20814,7 @@
         <v>5</v>
       </c>
       <c r="S224" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A224),"/"),B224)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/micropython/micropython</v>
       </c>
       <c r="T224" s="6" t="s">
@@ -20886,7 +20891,7 @@
         <v>49</v>
       </c>
       <c r="S225" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A225),"/"),B225)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/microsoft/ChakraCore</v>
       </c>
       <c r="T225" s="6" t="s">
@@ -20963,7 +20968,7 @@
         <v>32</v>
       </c>
       <c r="S226" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A226),"/"),B226)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/microsoft/CNTK</v>
       </c>
       <c r="T226" s="6" t="s">
@@ -21040,7 +21045,7 @@
         <v>84</v>
       </c>
       <c r="S227" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A227),"/"),B227)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/microsoft/TypeScript</v>
       </c>
       <c r="T227" s="6" t="s">
@@ -21117,7 +21122,7 @@
         <v>0</v>
       </c>
       <c r="S228" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A228),"/"),B228)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/microsoft/vscode</v>
       </c>
       <c r="T228" s="6" t="s">
@@ -21194,7 +21199,7 @@
         <v>117</v>
       </c>
       <c r="S229" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A229),"/"),B229)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/minio/minio</v>
       </c>
       <c r="T229" s="6" t="s">
@@ -21271,7 +21276,7 @@
         <v>28</v>
       </c>
       <c r="S230" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A230),"/"),B230)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/mirumee/saleor</v>
       </c>
       <c r="T230" s="6" t="s">
@@ -21348,7 +21353,7 @@
         <v>29</v>
       </c>
       <c r="S231" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A231),"/"),B231)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/mitmproxy/mitmproxy</v>
       </c>
       <c r="T231" s="6" t="s">
@@ -21425,7 +21430,7 @@
         <v>80</v>
       </c>
       <c r="S232" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A232),"/"),B232)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/moby/moby</v>
       </c>
       <c r="T232" s="8" t="s">
@@ -21502,7 +21507,7 @@
         <v>30</v>
       </c>
       <c r="S233" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A233),"/"),B233)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/mockito/mockito</v>
       </c>
       <c r="T233" s="6" t="s">
@@ -21579,7 +21584,7 @@
         <v>0</v>
       </c>
       <c r="S234" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A234),"/"),B234)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/mongodb/mongo</v>
       </c>
       <c r="T234" s="6" t="s">
@@ -21656,7 +21661,7 @@
         <v>4</v>
       </c>
       <c r="S235" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A235),"/"),B235)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/mongodb/node-mongodb-native</v>
       </c>
       <c r="T235" s="6" t="s">
@@ -21733,7 +21738,7 @@
         <v>0</v>
       </c>
       <c r="S236" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A236),"/"),B236)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/mono/mono</v>
       </c>
       <c r="T236" s="6" t="s">
@@ -21810,7 +21815,7 @@
         <v>14</v>
       </c>
       <c r="S237" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A237),"/"),B237)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/MonoGame/MonoGame</v>
       </c>
       <c r="T237" s="6" t="s">
@@ -21887,7 +21892,7 @@
         <v>8</v>
       </c>
       <c r="S238" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A238),"/"),B238)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/mopidy/mopidy</v>
       </c>
       <c r="T238" s="6" t="s">
@@ -21964,7 +21969,7 @@
         <v>30</v>
       </c>
       <c r="S239" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A239),"/"),B239)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/mozilla/pdf.js</v>
       </c>
       <c r="T239" s="6" t="s">
@@ -22041,7 +22046,7 @@
         <v>73</v>
       </c>
       <c r="S240" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A240),"/"),B240)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/mpv-player/mpv</v>
       </c>
       <c r="T240" s="6" t="s">
@@ -22118,7 +22123,7 @@
         <v>99</v>
       </c>
       <c r="S241" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A241),"/"),B241)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/mrdoob/three.js</v>
       </c>
       <c r="T241" s="6" t="s">
@@ -22195,7 +22200,7 @@
         <v>227</v>
       </c>
       <c r="S242" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A242),"/"),B242)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/mui-org/material-ui</v>
       </c>
       <c r="T242" s="6" t="s">
@@ -22272,7 +22277,7 @@
         <v>1</v>
       </c>
       <c r="S243" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A243),"/"),B243)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/NancyFx/Nancy</v>
       </c>
       <c r="T243" s="6" t="s">
@@ -22349,7 +22354,7 @@
         <v>17</v>
       </c>
       <c r="S244" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A244),"/"),B244)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/nasa/openmct</v>
       </c>
       <c r="T244" s="6" t="s">
@@ -22426,7 +22431,7 @@
         <v>39</v>
       </c>
       <c r="S245" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A245),"/"),B245)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/NativeScript/NativeScript</v>
       </c>
       <c r="T245" s="6" t="s">
@@ -22503,7 +22508,7 @@
         <v>30</v>
       </c>
       <c r="S246" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A246),"/"),B246)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/naver/pinpoint</v>
       </c>
       <c r="T246" s="6" t="s">
@@ -22580,7 +22585,7 @@
         <v>72</v>
       </c>
       <c r="S247" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A247),"/"),B247)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/neo4j/neo4j</v>
       </c>
       <c r="T247" s="6" t="s">
@@ -22657,7 +22662,7 @@
         <v>0</v>
       </c>
       <c r="S248" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A248),"/"),B248)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/NervJS/taro</v>
       </c>
       <c r="T248" s="6" t="s">
@@ -22734,7 +22739,7 @@
         <v>22</v>
       </c>
       <c r="S249" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A249),"/"),B249)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/netdata/netdata</v>
       </c>
       <c r="T249" s="6" t="s">
@@ -22811,7 +22816,7 @@
         <v>0</v>
       </c>
       <c r="S250" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A250),"/"),B250)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/netty/netty</v>
       </c>
       <c r="T250" s="6" t="s">
@@ -22888,7 +22893,7 @@
         <v>21</v>
       </c>
       <c r="S251" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A251),"/"),B251)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/networkx/networkx</v>
       </c>
       <c r="T251" s="6" t="s">
@@ -22965,7 +22970,7 @@
         <v>21</v>
       </c>
       <c r="S252" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A252),"/"),B252)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/nextcloud/server</v>
       </c>
       <c r="T252" s="6" t="s">
@@ -23042,7 +23047,7 @@
         <v>0</v>
       </c>
       <c r="S253" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A253),"/"),B253)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/nginx/nginx</v>
       </c>
       <c r="T253" s="6" t="s">
@@ -23119,7 +23124,7 @@
         <v>0</v>
       </c>
       <c r="S254" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A254),"/"),B254)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/nltk/nltk</v>
       </c>
       <c r="T254" s="6" t="s">
@@ -23196,7 +23201,7 @@
         <v>40</v>
       </c>
       <c r="S255" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A255),"/"),B255)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/NodeBB/NodeBB</v>
       </c>
       <c r="T255" s="6" t="s">
@@ -23273,7 +23278,7 @@
         <v>118</v>
       </c>
       <c r="S256" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A256),"/"),B256)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/nodejs/node</v>
       </c>
       <c r="T256" s="6" t="s">
@@ -23350,7 +23355,7 @@
         <v>47</v>
       </c>
       <c r="S257" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A257),"/"),B257)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/numenta/nupic</v>
       </c>
       <c r="T257" s="6" t="s">
@@ -23427,7 +23432,7 @@
         <v>38</v>
       </c>
       <c r="S258" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A258),"/"),B258)</f>
+        <f t="shared" si="3"/>
         <v>http://www.github.com/numpy/numpy</v>
       </c>
       <c r="T258" s="6" t="s">
@@ -23504,7 +23509,7 @@
         <v>53</v>
       </c>
       <c r="S259" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A259),"/"),B259)</f>
+        <f t="shared" ref="S259:S322" si="4">CONCATENATE(CONCATENATE(CONCATENATE("http://www.github.com/",A259),"/"),B259)</f>
         <v>http://www.github.com/nylas/nylas-mail</v>
       </c>
       <c r="T259" s="6" t="s">
@@ -23581,7 +23586,7 @@
         <v>94</v>
       </c>
       <c r="S260" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A260),"/"),B260)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/obsproject/obs-studio</v>
       </c>
       <c r="T260" s="6" t="s">
@@ -23658,7 +23663,7 @@
         <v>61</v>
       </c>
       <c r="S261" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A261),"/"),B261)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/ocornut/imgui</v>
       </c>
       <c r="T261" s="6" t="s">
@@ -23735,7 +23740,7 @@
         <v>0</v>
       </c>
       <c r="S262" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A262),"/"),B262)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/odoo/odoo</v>
       </c>
       <c r="T262" s="6" t="s">
@@ -23812,7 +23817,7 @@
         <v>2781</v>
       </c>
       <c r="S263" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A263),"/"),B263)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/OfficeDev/office-ui-fabric-react</v>
       </c>
       <c r="T263" s="6" t="s">
@@ -23889,7 +23894,7 @@
         <v>58</v>
       </c>
       <c r="S264" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A264),"/"),B264)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/OnsenUI/OnsenUI</v>
       </c>
       <c r="T264" s="6" t="s">
@@ -23966,7 +23971,7 @@
         <v>22</v>
       </c>
       <c r="S265" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A265),"/"),B265)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/opencart/opencart</v>
       </c>
       <c r="T265" s="6" t="s">
@@ -24043,7 +24048,7 @@
         <v>38</v>
       </c>
       <c r="S266" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A266),"/"),B266)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/opencv/opencv</v>
       </c>
       <c r="T266" s="6" t="s">
@@ -24120,7 +24125,7 @@
         <v>0</v>
       </c>
       <c r="S267" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A267),"/"),B267)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/openframeworks/openFrameworks</v>
       </c>
       <c r="T267" s="6" t="s">
@@ -24197,7 +24202,7 @@
         <v>82</v>
       </c>
       <c r="S268" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A268),"/"),B268)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/openlayers/openlayers</v>
       </c>
       <c r="T268" s="6" t="s">
@@ -24274,7 +24279,7 @@
         <v>73</v>
       </c>
       <c r="S269" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A269),"/"),B269)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/OpenRA/OpenRA</v>
       </c>
       <c r="T269" s="6" t="s">
@@ -24351,7 +24356,7 @@
         <v>15</v>
       </c>
       <c r="S270" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A270),"/"),B270)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/OpenRCT2/OpenRCT2</v>
       </c>
       <c r="T270" s="6" t="s">
@@ -24428,7 +24433,7 @@
         <v>59</v>
       </c>
       <c r="S271" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A271),"/"),B271)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/openshift/origin</v>
       </c>
       <c r="T271" s="6" t="s">
@@ -24505,7 +24510,7 @@
         <v>0</v>
       </c>
       <c r="S272" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A272),"/"),B272)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/openssl/openssl</v>
       </c>
       <c r="T272" s="6" t="s">
@@ -24582,7 +24587,7 @@
         <v>28</v>
       </c>
       <c r="S273" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A273),"/"),B273)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/oracle/graal</v>
       </c>
       <c r="T273" s="6" t="s">
@@ -24659,7 +24664,7 @@
         <v>96</v>
       </c>
       <c r="S274" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A274),"/"),B274)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/osquery/osquery</v>
       </c>
       <c r="T274" s="6" t="s">
@@ -24736,7 +24741,7 @@
         <v>0</v>
       </c>
       <c r="S275" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A275),"/"),B275)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/owncloud/core</v>
       </c>
       <c r="T275" s="6" t="s">
@@ -24813,7 +24818,7 @@
         <v>25</v>
       </c>
       <c r="S276" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A276),"/"),B276)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/PaddlePaddle/Paddle</v>
       </c>
       <c r="T276" s="6" t="s">
@@ -24890,7 +24895,7 @@
         <v>51</v>
       </c>
       <c r="S277" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A277),"/"),B277)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/pandas-dev/pandas</v>
       </c>
       <c r="T277" s="6" t="s">
@@ -24967,7 +24972,7 @@
         <v>15</v>
       </c>
       <c r="S278" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A278),"/"),B278)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/paperjs/paper.js</v>
       </c>
       <c r="T278" s="6" t="s">
@@ -25044,7 +25049,7 @@
         <v>0</v>
       </c>
       <c r="S279" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A279),"/"),B279)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/phacility/phabricator</v>
       </c>
       <c r="T279" s="6" t="s">
@@ -25121,7 +25126,7 @@
         <v>65</v>
       </c>
       <c r="S280" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A280),"/"),B280)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/phalcon/cphalcon</v>
       </c>
       <c r="T280" s="6" t="s">
@@ -25198,7 +25203,7 @@
         <v>89</v>
       </c>
       <c r="S281" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A281),"/"),B281)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/photonstorm/phaser</v>
       </c>
       <c r="T281" s="6" t="s">
@@ -25275,7 +25280,7 @@
         <v>0</v>
       </c>
       <c r="S282" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A282),"/"),B282)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/php/php-src</v>
       </c>
       <c r="T282" s="6" t="s">
@@ -25352,7 +25357,7 @@
         <v>69</v>
       </c>
       <c r="S283" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A283),"/"),B283)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/pingcap/tidb</v>
       </c>
       <c r="T283" s="6" t="s">
@@ -25429,7 +25434,7 @@
         <v>98</v>
       </c>
       <c r="S284" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A284),"/"),B284)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/pixijs/pixi.js</v>
       </c>
       <c r="T284" s="6" t="s">
@@ -25506,7 +25511,7 @@
         <v>141</v>
       </c>
       <c r="S285" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A285),"/"),B285)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/plotly/plotly.js</v>
       </c>
       <c r="T285" s="6" t="s">
@@ -25583,7 +25588,7 @@
         <v>0</v>
       </c>
       <c r="S286" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A286),"/"),B286)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/postgres/postgres</v>
       </c>
       <c r="T286" s="6" t="s">
@@ -25660,7 +25665,7 @@
         <v>57</v>
       </c>
       <c r="S287" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A287),"/"),B287)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/PowerShell/PowerShell</v>
       </c>
       <c r="T287" s="6" t="s">
@@ -25737,7 +25742,7 @@
         <v>0</v>
       </c>
       <c r="S288" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A288),"/"),B288)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/prestodb/presto</v>
       </c>
       <c r="T288" s="8" t="s">
@@ -25814,7 +25819,7 @@
         <v>127</v>
       </c>
       <c r="S289" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A289),"/"),B289)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/primefaces/primeng</v>
       </c>
       <c r="T289" s="6" t="s">
@@ -25891,7 +25896,7 @@
         <v>65</v>
       </c>
       <c r="S290" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A290),"/"),B290)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/processing/p5.js</v>
       </c>
       <c r="T290" s="6" t="s">
@@ -25968,7 +25973,7 @@
         <v>47</v>
       </c>
       <c r="S291" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A291),"/"),B291)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/processing/processing</v>
       </c>
       <c r="T291" s="6" t="s">
@@ -26045,7 +26050,7 @@
         <v>120</v>
       </c>
       <c r="S292" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A292),"/"),B292)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/prometheus/prometheus</v>
       </c>
       <c r="T292" s="6" t="s">
@@ -26122,7 +26127,7 @@
         <v>34</v>
       </c>
       <c r="S293" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A293),"/"),B293)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/protocolbuffers/protobuf</v>
       </c>
       <c r="T293" s="6" t="s">
@@ -26199,7 +26204,7 @@
         <v>0</v>
       </c>
       <c r="S294" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A294),"/"),B294)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/psf/requests</v>
       </c>
       <c r="T294" s="6" t="s">
@@ -26276,7 +26281,7 @@
         <v>9</v>
       </c>
       <c r="S295" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A295),"/"),B295)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/ptmt/react-native-macos</v>
       </c>
       <c r="T295" s="6" t="s">
@@ -26353,7 +26358,7 @@
         <v>0</v>
       </c>
       <c r="S296" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A296),"/"),B296)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/puppetlabs/puppet</v>
       </c>
       <c r="T296" s="6" t="s">
@@ -26430,7 +26435,7 @@
         <v>23</v>
       </c>
       <c r="S297" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A297),"/"),B297)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/pyinstaller/pyinstaller</v>
       </c>
       <c r="T297" s="6" t="s">
@@ -26507,7 +26512,7 @@
         <v>0</v>
       </c>
       <c r="S298" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A298),"/"),B298)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/pypa/pip</v>
       </c>
       <c r="T298" s="6" t="s">
@@ -26584,7 +26589,7 @@
         <v>6</v>
       </c>
       <c r="S299" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A299),"/"),B299)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/pypa/pipenv</v>
       </c>
       <c r="T299" s="6" t="s">
@@ -26661,7 +26666,7 @@
         <v>0</v>
       </c>
       <c r="S300" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A300),"/"),B300)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/python/cpython</v>
       </c>
       <c r="T300" s="6" t="s">
@@ -26738,7 +26743,7 @@
         <v>0</v>
       </c>
       <c r="S301" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A301),"/"),B301)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/python/mypy</v>
       </c>
       <c r="T301" s="6" t="s">
@@ -26815,7 +26820,7 @@
         <v>24</v>
       </c>
       <c r="S302" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A302),"/"),B302)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/python-pillow/Pillow</v>
       </c>
       <c r="T302" s="6" t="s">
@@ -26892,7 +26897,7 @@
         <v>22</v>
       </c>
       <c r="S303" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A303),"/"),B303)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/pytorch/pytorch</v>
       </c>
       <c r="T303" s="6" t="s">
@@ -26969,7 +26974,7 @@
         <v>0</v>
       </c>
       <c r="S304" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A304),"/"),B304)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/qbittorrent/qBittorrent</v>
       </c>
       <c r="T304" s="6" t="s">
@@ -27046,7 +27051,7 @@
         <v>11</v>
       </c>
       <c r="S305" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A305),"/"),B305)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/quantopian/zipline</v>
       </c>
       <c r="T305" s="6" t="s">
@@ -27123,7 +27128,7 @@
         <v>142</v>
       </c>
       <c r="S306" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A306),"/"),B306)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/quasarframework/quasar</v>
       </c>
       <c r="T306" s="6" t="s">
@@ -27200,7 +27205,7 @@
         <v>81</v>
       </c>
       <c r="S307" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A307),"/"),B307)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/quilljs/quill</v>
       </c>
       <c r="T307" s="6" t="s">
@@ -27277,7 +27282,7 @@
         <v>0</v>
       </c>
       <c r="S308" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A308),"/"),B308)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/ractivejs/ractive</v>
       </c>
       <c r="T308" s="6" t="s">
@@ -27354,7 +27359,7 @@
         <v>50</v>
       </c>
       <c r="S309" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A309),"/"),B309)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/radare/radare2</v>
       </c>
       <c r="T309" s="6" t="s">
@@ -27431,7 +27436,7 @@
         <v>6</v>
       </c>
       <c r="S310" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A310),"/"),B310)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/rails/rails</v>
       </c>
       <c r="T310" s="6" t="s">
@@ -27508,7 +27513,7 @@
         <v>0</v>
       </c>
       <c r="S311" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A311),"/"),B311)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/rapid7/metasploit-framework</v>
       </c>
       <c r="T311" s="6" t="s">
@@ -27585,7 +27590,7 @@
         <v>2</v>
       </c>
       <c r="S312" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A312),"/"),B312)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/RasaHQ/rasa</v>
       </c>
       <c r="T312" s="6" t="s">
@@ -27662,7 +27667,7 @@
         <v>0</v>
       </c>
       <c r="S313" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A313),"/"),B313)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/raspberrypi/linux</v>
       </c>
       <c r="T313" s="6" t="s">
@@ -27739,7 +27744,7 @@
         <v>125</v>
       </c>
       <c r="S314" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A314),"/"),B314)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/reactioncommerce/reaction</v>
       </c>
       <c r="T314" s="6" t="s">
@@ -27816,7 +27821,7 @@
         <v>178</v>
       </c>
       <c r="S315" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A315),"/"),B315)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/ReactiveX/RxJava</v>
       </c>
       <c r="T315" s="6" t="s">
@@ -27893,7 +27898,7 @@
         <v>5</v>
       </c>
       <c r="S316" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A316),"/"),B316)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/reactos/reactos</v>
       </c>
       <c r="T316" s="6" t="s">
@@ -27970,7 +27975,7 @@
         <v>0</v>
       </c>
       <c r="S317" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A317),"/"),B317)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/readthedocs/readthedocs.org</v>
       </c>
       <c r="T317" s="6" t="s">
@@ -28047,7 +28052,7 @@
         <v>0</v>
       </c>
       <c r="S318" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A318),"/"),B318)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/realm/realm-java</v>
       </c>
       <c r="T318" s="6" t="s">
@@ -28124,7 +28129,7 @@
         <v>70</v>
       </c>
       <c r="S319" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A319),"/"),B319)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/redisson/redisson</v>
       </c>
       <c r="T319" s="6" t="s">
@@ -28201,7 +28206,7 @@
         <v>67</v>
       </c>
       <c r="S320" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A320),"/"),B320)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/rethinkdb/rethinkdb</v>
       </c>
       <c r="T320" s="6" t="s">
@@ -28278,7 +28283,7 @@
         <v>65</v>
       </c>
       <c r="S321" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A321),"/"),B321)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/rkt/rkt</v>
       </c>
       <c r="T321" s="6" t="s">
@@ -28355,7 +28360,7 @@
         <v>0</v>
       </c>
       <c r="S322" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A322),"/"),B322)</f>
+        <f t="shared" si="4"/>
         <v>http://www.github.com/RMerl/asuswrt-merlin</v>
       </c>
       <c r="T322" s="17" t="s">
@@ -28432,7 +28437,7 @@
         <v>270</v>
       </c>
       <c r="S323" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A323),"/"),B323)</f>
+        <f t="shared" ref="S323:S386" si="5">CONCATENATE(CONCATENATE(CONCATENATE("http://www.github.com/",A323),"/"),B323)</f>
         <v>http://www.github.com/RocketChat/Rocket.Chat</v>
       </c>
       <c r="T323" s="6" t="s">
@@ -28509,7 +28514,7 @@
         <v>8</v>
       </c>
       <c r="S324" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A324),"/"),B324)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/RPCS3/rpcs3</v>
       </c>
       <c r="T324" s="6" t="s">
@@ -28586,7 +28591,7 @@
         <v>84</v>
       </c>
       <c r="S325" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A325),"/"),B325)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/rubocop-hq/rubocop</v>
       </c>
       <c r="T325" s="6" t="s">
@@ -28663,7 +28668,7 @@
         <v>0</v>
       </c>
       <c r="S326" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A326),"/"),B326)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/ruby/ruby</v>
       </c>
       <c r="T326" s="6" t="s">
@@ -28740,7 +28745,7 @@
         <v>130</v>
       </c>
       <c r="S327" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A327),"/"),B327)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/saltstack/salt</v>
       </c>
       <c r="T327" s="6" t="s">
@@ -28817,7 +28822,7 @@
         <v>0</v>
       </c>
       <c r="S328" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A328),"/"),B328)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/samuelclay/NewsBlur</v>
       </c>
       <c r="T328" s="6" t="s">
@@ -28894,7 +28899,7 @@
         <v>0</v>
       </c>
       <c r="S329" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A329),"/"),B329)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/sandstorm-io/sandstorm</v>
       </c>
       <c r="T329" s="6" t="s">
@@ -28971,7 +28976,7 @@
         <v>14</v>
       </c>
       <c r="S330" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A330),"/"),B330)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/scikit-learn/scikit-learn</v>
       </c>
       <c r="T330" s="6" t="s">
@@ -29048,7 +29053,7 @@
         <v>33</v>
       </c>
       <c r="S331" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A331),"/"),B331)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/scipy/scipy</v>
       </c>
       <c r="T331" s="6" t="s">
@@ -29125,7 +29130,7 @@
         <v>10</v>
       </c>
       <c r="S332" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A332),"/"),B332)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/scrapy/scrapy</v>
       </c>
       <c r="T332" s="6" t="s">
@@ -29202,7 +29207,7 @@
         <v>0</v>
       </c>
       <c r="S333" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A333),"/"),B333)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/scylladb/scylla</v>
       </c>
       <c r="T333" s="6" t="s">
@@ -29279,7 +29284,7 @@
         <v>33</v>
       </c>
       <c r="S334" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A334),"/"),B334)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/sebastianbergmann/phpunit</v>
       </c>
       <c r="T334" s="6" t="s">
@@ -29356,7 +29361,7 @@
         <v>27</v>
       </c>
       <c r="S335" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A335),"/"),B335)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/SeleniumHQ/selenium</v>
       </c>
       <c r="T335" s="6" t="s">
@@ -29433,7 +29438,7 @@
         <v>153</v>
       </c>
       <c r="S336" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A336),"/"),B336)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/Semantic-Org/Semantic-UI</v>
       </c>
       <c r="T336" s="6" t="s">
@@ -29510,7 +29515,7 @@
         <v>296</v>
       </c>
       <c r="S337" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A337),"/"),B337)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/sequelize/sequelize</v>
       </c>
       <c r="T337" s="6" t="s">
@@ -29587,7 +29592,7 @@
         <v>118</v>
       </c>
       <c r="S338" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A338),"/"),B338)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/serverless/serverless</v>
       </c>
       <c r="T338" s="6" t="s">
@@ -29664,7 +29669,7 @@
         <v>61</v>
       </c>
       <c r="S339" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A339),"/"),B339)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/ShareX/ShareX</v>
       </c>
       <c r="T339" s="6" t="s">
@@ -29741,7 +29746,7 @@
         <v>110</v>
       </c>
       <c r="S340" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A340),"/"),B340)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/spree/spree</v>
       </c>
       <c r="T340" s="6" t="s">
@@ -29818,7 +29823,7 @@
         <v>34</v>
       </c>
       <c r="S341" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A341),"/"),B341)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/spring-projects/spring-boot</v>
       </c>
       <c r="T341" s="6" t="s">
@@ -29895,7 +29900,7 @@
         <v>157</v>
       </c>
       <c r="S342" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A342),"/"),B342)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/spring-projects/spring-framework</v>
       </c>
       <c r="T342" s="6" t="s">
@@ -29972,7 +29977,7 @@
         <v>4</v>
       </c>
       <c r="S343" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A343),"/"),B343)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/sqlmapproject/sqlmap</v>
       </c>
       <c r="T343" s="6" t="s">
@@ -30049,7 +30054,7 @@
         <v>73</v>
       </c>
       <c r="S344" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A344),"/"),B344)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/squizlabs/PHP_CodeSniffer</v>
       </c>
       <c r="T344" s="6" t="s">
@@ -30126,7 +30131,7 @@
         <v>0</v>
       </c>
       <c r="S345" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A345),"/"),B345)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/stanfordnlp/CoreNLP</v>
       </c>
       <c r="T345" s="6" t="s">
@@ -30203,7 +30208,7 @@
         <v>320</v>
       </c>
       <c r="S346" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A346),"/"),B346)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/storybookjs/storybook</v>
       </c>
       <c r="T346" s="6" t="s">
@@ -30280,7 +30285,7 @@
         <v>95</v>
       </c>
       <c r="S347" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A347),"/"),B347)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/strapi/strapi</v>
       </c>
       <c r="T347" s="6" t="s">
@@ -30357,7 +30362,7 @@
         <v>40</v>
       </c>
       <c r="S348" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A348),"/"),B348)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/swaywm/sway</v>
       </c>
       <c r="T348" s="6" t="s">
@@ -30434,7 +30439,7 @@
         <v>171</v>
       </c>
       <c r="S349" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A349),"/"),B349)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/swoole/swoole-src</v>
       </c>
       <c r="T349" s="6" t="s">
@@ -30511,7 +30516,7 @@
         <v>101</v>
       </c>
       <c r="S350" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A350),"/"),B350)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/Sylius/Sylius</v>
       </c>
       <c r="T350" s="6" t="s">
@@ -30588,7 +30593,7 @@
         <v>187</v>
       </c>
       <c r="S351" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A351),"/"),B351)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/symfony/symfony</v>
       </c>
       <c r="T351" s="6" t="s">
@@ -30665,7 +30670,7 @@
         <v>24</v>
       </c>
       <c r="S352" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A352),"/"),B352)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/sympy/sympy</v>
       </c>
       <c r="T352" s="6" t="s">
@@ -30742,7 +30747,7 @@
         <v>166</v>
       </c>
       <c r="S353" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A353),"/"),B353)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/syncthing/syncthing</v>
       </c>
       <c r="T353" s="6" t="s">
@@ -30819,7 +30824,7 @@
         <v>27</v>
       </c>
       <c r="S354" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A354),"/"),B354)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/systemd/systemd</v>
       </c>
       <c r="T354" s="6" t="s">
@@ -30896,7 +30901,7 @@
         <v>385</v>
       </c>
       <c r="S355" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A355),"/"),B355)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/telegramdesktop/tdesktop</v>
       </c>
       <c r="T355" s="6" t="s">
@@ -30973,7 +30978,7 @@
         <v>76</v>
       </c>
       <c r="S356" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A356),"/"),B356)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/Tencent/omi</v>
       </c>
       <c r="T356" s="6" t="s">
@@ -31050,7 +31055,7 @@
         <v>84</v>
       </c>
       <c r="S357" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A357),"/"),B357)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/tensorflow/tensorflow</v>
       </c>
       <c r="T357" s="6" t="s">
@@ -31127,7 +31132,7 @@
         <v>0</v>
       </c>
       <c r="S358" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A358),"/"),B358)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/Theano/Theano</v>
       </c>
       <c r="T358" s="6" t="s">
@@ -31204,7 +31209,7 @@
         <v>0</v>
       </c>
       <c r="S359" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A359),"/"),B359)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/tinymce/tinymce</v>
       </c>
       <c r="T359" s="6" t="s">
@@ -31281,7 +31286,7 @@
         <v>0</v>
       </c>
       <c r="S360" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A360),"/"),B360)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/tldr-pages/tldr</v>
       </c>
       <c r="T360" s="6" t="s">
@@ -31358,7 +31363,7 @@
         <v>126</v>
       </c>
       <c r="S361" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A361),"/"),B361)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/tootsuite/mastodon</v>
       </c>
       <c r="T361" s="6" t="s">
@@ -31435,7 +31440,7 @@
         <v>0</v>
       </c>
       <c r="S362" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A362),"/"),B362)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/torvalds/linux</v>
       </c>
       <c r="T362" s="6" t="s">
@@ -31512,7 +31517,7 @@
         <v>23</v>
       </c>
       <c r="S363" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A363),"/"),B363)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/transloadit/uppy</v>
       </c>
       <c r="T363" s="6" t="s">
@@ -31589,7 +31594,7 @@
         <v>27</v>
       </c>
       <c r="S364" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A364),"/"),B364)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/TrinityCore/TrinityCore</v>
       </c>
       <c r="T364" s="6" t="s">
@@ -31666,7 +31671,7 @@
         <v>74</v>
       </c>
       <c r="S365" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A365),"/"),B365)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/trufflesuite/truffle</v>
       </c>
       <c r="T365" s="6" t="s">
@@ -31743,7 +31748,7 @@
         <v>264</v>
       </c>
       <c r="S366" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A366),"/"),B366)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/TryGhost/Ghost</v>
       </c>
       <c r="T366" s="6" t="s">
@@ -31820,7 +31825,7 @@
         <v>55</v>
       </c>
       <c r="S367" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A367),"/"),B367)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/twbs/bootstrap</v>
       </c>
       <c r="T367" s="6" t="s">
@@ -31897,7 +31902,7 @@
         <v>0</v>
       </c>
       <c r="S368" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A368),"/"),B368)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/v8/v8</v>
       </c>
       <c r="T368" s="6" t="s">
@@ -31974,7 +31979,7 @@
         <v>94</v>
       </c>
       <c r="S369" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A369),"/"),B369)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/vega/vega</v>
       </c>
       <c r="T369" s="6" t="s">
@@ -32051,7 +32056,7 @@
         <v>0</v>
       </c>
       <c r="S370" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A370),"/"),B370)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/videolan/vlc</v>
       </c>
       <c r="T370" s="6" t="s">
@@ -32128,7 +32133,7 @@
         <v>20</v>
       </c>
       <c r="S371" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A371),"/"),B371)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/vitessio/vitess</v>
       </c>
       <c r="T371" s="6" t="s">
@@ -32205,7 +32210,7 @@
         <v>9</v>
       </c>
       <c r="S372" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A372),"/"),B372)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/VowpalWabbit/vowpal_wabbit</v>
       </c>
       <c r="T372" s="6" t="s">
@@ -32282,7 +32287,7 @@
         <v>261</v>
       </c>
       <c r="S373" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A373),"/"),B373)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/vuetifyjs/vuetify</v>
       </c>
       <c r="T373" s="6" t="s">
@@ -32359,7 +32364,7 @@
         <v>54</v>
       </c>
       <c r="S374" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A374),"/"),B374)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/VulcanJS/Vulcan</v>
       </c>
       <c r="T374" s="6" t="s">
@@ -32436,7 +32441,7 @@
         <v>106</v>
       </c>
       <c r="S375" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A375),"/"),B375)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/wagtail/wagtail</v>
       </c>
       <c r="T375" s="6" t="s">
@@ -32513,7 +32518,7 @@
         <v>66</v>
       </c>
       <c r="S376" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A376),"/"),B376)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/weaveworks/weave</v>
       </c>
       <c r="T376" s="6" t="s">
@@ -32590,7 +32595,7 @@
         <v>176</v>
       </c>
       <c r="S377" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A377),"/"),B377)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/webpack/webpack</v>
       </c>
       <c r="T377" s="6" t="s">
@@ -32667,7 +32672,7 @@
         <v>159</v>
       </c>
       <c r="S378" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A378),"/"),B378)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/withspectrum/spectrum</v>
       </c>
       <c r="T378" s="6" t="s">
@@ -32744,7 +32749,7 @@
         <v>154</v>
       </c>
       <c r="S379" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A379),"/"),B379)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/woocommerce/woocommerce</v>
       </c>
       <c r="T379" s="6" t="s">
@@ -32821,7 +32826,7 @@
         <v>69</v>
       </c>
       <c r="S380" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A380),"/"),B380)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/WordPress/gutenberg</v>
       </c>
       <c r="T380" s="6" t="s">
@@ -32898,7 +32903,7 @@
         <v>0</v>
       </c>
       <c r="S381" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A381),"/"),B381)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/WordPress/WordPress</v>
       </c>
       <c r="T381" s="6" t="s">
@@ -32975,7 +32980,7 @@
         <v>126</v>
       </c>
       <c r="S382" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A382),"/"),B382)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/xbmc/xbmc</v>
       </c>
       <c r="T382" s="6" t="s">
@@ -33052,7 +33057,7 @@
         <v>0</v>
       </c>
       <c r="S383" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A383),"/"),B383)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/yandex/ClickHouse</v>
       </c>
       <c r="T383" s="6" t="s">
@@ -33129,7 +33134,7 @@
         <v>40</v>
       </c>
       <c r="S384" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A384),"/"),B384)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/yiisoft/yii2</v>
       </c>
       <c r="T384" s="6" t="s">
@@ -33206,7 +33211,7 @@
         <v>0</v>
       </c>
       <c r="S385" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A385),"/"),B385)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/YMFE/yapi</v>
       </c>
       <c r="T385" s="6" t="s">
@@ -33283,7 +33288,7 @@
         <v>272</v>
       </c>
       <c r="S386" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A386),"/"),B386)</f>
+        <f t="shared" si="5"/>
         <v>http://www.github.com/ytdl-org/youtube-dl</v>
       </c>
       <c r="T386" s="6" t="s">
@@ -33360,7 +33365,7 @@
         <v>0</v>
       </c>
       <c r="S387" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A387),"/"),B387)</f>
+        <f t="shared" ref="S387:S390" si="6">CONCATENATE(CONCATENATE(CONCATENATE("http://www.github.com/",A387),"/"),B387)</f>
         <v>http://www.github.com/yuzu-emu/yuzu</v>
       </c>
       <c r="T387" s="6" t="s">
@@ -33437,7 +33442,7 @@
         <v>124</v>
       </c>
       <c r="S388" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A388),"/"),B388)</f>
+        <f t="shared" si="6"/>
         <v>http://www.github.com/zaproxy/zaproxy</v>
       </c>
       <c r="T388" s="6" t="s">
@@ -33514,7 +33519,7 @@
         <v>10</v>
       </c>
       <c r="S389" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A389),"/"),B389)</f>
+        <f t="shared" si="6"/>
         <v>http://www.github.com/zeromq/libzmq</v>
       </c>
       <c r="T389" s="6" t="s">
@@ -33584,7 +33589,7 @@
         <v>36</v>
       </c>
       <c r="S390" s="5" t="str">
-        <f>_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("http://www.github.com/",A390),"/"),B390)</f>
+        <f t="shared" si="6"/>
         <v>http://www.github.com/zulip/zulip</v>
       </c>
       <c r="T390" s="6" t="s">
@@ -56703,19 +56708,19 @@
       <c r="AD1112" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W1110" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W1110">
+  <autoFilter ref="A1:W1110">
+    <sortState ref="A2:W1110">
       <sortCondition ref="A1:A1110"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W390">
+  <sortState ref="A2:W390">
     <sortCondition ref="A2:A390"/>
     <sortCondition ref="B2:B390"/>
   </sortState>
   <customSheetViews>
     <customSheetView guid="{5C673459-04D6-4823-9839-02892B7E791C}" filter="1" showAutoFilter="1">
       <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-      <autoFilter ref="U1:U1112" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
+      <autoFilter ref="U1:U1112"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="T2:T1112">

</xml_diff>